<commit_message>
Revert "Revert "Bryce's Timesheet""
This reverts commit 2f77c0e54799006fc942aa2b7c43ff9394678a77.
</commit_message>
<xml_diff>
--- a/Administration/timecards/IndTimeSheet_TEMPLATE.xlsx
+++ b/Administration/timecards/IndTimeSheet_TEMPLATE.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\Flynet\Administration\timecards\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="345" windowWidth="18705" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -85,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="m/d"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -113,6 +118,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -344,7 +350,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -525,6 +531,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -572,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -822,7 +831,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>